<commit_message>
Excelfiles und reader verbesserung
</commit_message>
<xml_diff>
--- a/openEAR-0.1.0 Kopie/SmileArchiv/None.xlsx
+++ b/openEAR-0.1.0 Kopie/SmileArchiv/None.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:B21"/>
+  <dimension ref="A3:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,7 +426,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>7.758323</v>
+        <v>21.487739</v>
+      </c>
+      <c r="C3" t="n">
+        <v>33.449434</v>
+      </c>
+      <c r="D3" t="n">
+        <v>36.351233</v>
+      </c>
+      <c r="E3" t="n">
+        <v>39.081447</v>
+      </c>
+      <c r="F3" t="n">
+        <v>42.737567</v>
       </c>
     </row>
     <row r="4">
@@ -434,7 +446,19 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>0.19</v>
+        <v>0.24</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.04</v>
       </c>
     </row>
     <row r="5">
@@ -442,7 +466,19 @@
         <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>0.08</v>
+        <v>0.05</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.02</v>
       </c>
     </row>
     <row r="6">
@@ -450,7 +486,19 @@
         <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>0.013417</v>
+        <v>0.037014</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.030728</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.010464</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.010177</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.01817</v>
       </c>
     </row>
     <row r="7">
@@ -458,7 +506,19 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>0.026184</v>
+        <v>0.132336</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.06342</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.248894</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.46513</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.494593</v>
       </c>
     </row>
     <row r="8">
@@ -466,7 +526,19 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>0.513231</v>
+        <v>0.083643</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.08955200000000001</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.155616</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.054392</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.10753</v>
       </c>
     </row>
     <row r="9">
@@ -474,7 +546,19 @@
         <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>0.326776</v>
+        <v>0.468956</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.518135</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.198485</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.015336</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.013869</v>
       </c>
     </row>
     <row r="10">
@@ -482,7 +566,19 @@
         <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>0.031667</v>
+        <v>0.086788</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.082331</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.051939</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.011576</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.014201</v>
       </c>
     </row>
     <row r="11">
@@ -490,7 +586,19 @@
         <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>0.018464</v>
+        <v>0.132094</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.059683</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.282421</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.335834</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.263771</v>
       </c>
     </row>
     <row r="12">
@@ -498,7 +606,19 @@
         <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>0.07026200000000001</v>
+        <v>0.05917</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.156151</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.052179</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.107554</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.087865</v>
       </c>
     </row>
     <row r="13">
@@ -506,7 +626,19 @@
         <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>0.784096</v>
+        <v>0.758576</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.834748</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.417218</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.152476</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.074265</v>
       </c>
     </row>
     <row r="14">
@@ -514,7 +646,19 @@
         <v>0</v>
       </c>
       <c r="B14" t="n">
-        <v>0.06242</v>
+        <v>0.082551</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.053798</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.096844</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.359644</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.192006</v>
       </c>
     </row>
     <row r="15">
@@ -522,7 +666,19 @@
         <v>0</v>
       </c>
       <c r="B15" t="n">
-        <v>0.032906</v>
+        <v>0.017988</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.006497</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.281691</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.287962</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.556658</v>
       </c>
     </row>
     <row r="16">
@@ -530,7 +686,19 @@
         <v>0</v>
       </c>
       <c r="B16" t="n">
-        <v>0.028809</v>
+        <v>0.01245</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.016658</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.023613</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.015358</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.007247</v>
       </c>
     </row>
     <row r="17">
@@ -538,7 +706,19 @@
         <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>0.08395</v>
+        <v>0.123306</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.081051</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.029601</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.129525</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.114049</v>
       </c>
     </row>
     <row r="18">
@@ -546,7 +726,19 @@
         <v>0</v>
       </c>
       <c r="B18" t="n">
-        <v>0.007820000000000001</v>
+        <v>0.005129</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.007248</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.151031</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.055035</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.055776</v>
       </c>
     </row>
     <row r="19">
@@ -554,7 +746,19 @@
         <v>0</v>
       </c>
       <c r="B19" t="n">
-        <v>0.026182</v>
+        <v>0.007336</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.038562</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.00651</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.00468</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.00311</v>
       </c>
     </row>
     <row r="20">
@@ -562,7 +766,19 @@
         <v>0</v>
       </c>
       <c r="B20" t="n">
-        <v>0.799731</v>
+        <v>0.873723</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.765254</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.757493</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.547498</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.897111</v>
       </c>
     </row>
     <row r="21">
@@ -570,7 +786,280 @@
         <v>0</v>
       </c>
       <c r="B21" t="n">
-        <v>0.174087</v>
+        <v>0.118941</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.196184</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.235997</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.447822</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.09977999999999999</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0.06743775</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>0.29886375</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>0.06159575</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0.30633225</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0.09225925</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>0.1257095</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>0.04780175</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>0.06743775</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.29886375</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.06159575</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.30633225</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.09225925</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.1257095</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.04780175</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0.5911573631587611</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>0.006152395</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>0.306738115</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>0.23492557</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0.179188181</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>0.272995739</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>0.5911573631587611</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0.006152395</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.306738115</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.23492557</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.179188181</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.272995739</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>0.139625</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0.08347500000000002</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0.018777915</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0.29610506375</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>0.098933745</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0.215002365</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>0.0449965425</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>0.2306732825</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>0.0955102625</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0.018777915</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.29610506375</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.098933745</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.215002365</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.0449965425</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.2306732825</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.0955102625</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0.41376086375</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>0.1723875250000001</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>0.24294294375</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>0.0160233675</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>0.0912479375</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>0.06363703125000002</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>0.41376086375</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.1723875250000001</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.24294294375</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.0160233675</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.0912479375</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.06363703125000002</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>0.01227494</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>0.7386553650000001</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>0.24906986125</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>0.6552198814457406</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>0.7137426433807432</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>0.6844812624132419</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>0.618397460625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>